<commit_message>
Added 'Stored in refrigerator' as an option for 'preparation condition'
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="137">
   <si>
     <t>source_id</t>
   </si>
@@ -305,30 +305,30 @@
     <t>http://purl.obolibrary.org/obo/OBI_0100046</t>
   </si>
   <si>
-    <t>NBF (Neutral Buffered Formalin)</t>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
+  </si>
+  <si>
+    <t>Allprotect tissue reagent (ALL)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000118</t>
+  </si>
+  <si>
+    <t>CLARITY hydrogel</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000134</t>
+  </si>
+  <si>
+    <t>Neutral Buffered Formalin (NBF)</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBIB_0000213</t>
   </si>
   <si>
-    <t>Ethanol</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
-  </si>
-  <si>
-    <t>Allprotect tissue reagent (ALL)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000118</t>
-  </si>
-  <si>
-    <t>CLARITY hydrogel</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000134</t>
-  </si>
-  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -470,6 +470,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C187069</t>
   </si>
   <si>
+    <t>Stored in refrigerator</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000104</t>
+  </si>
+  <si>
     <t>processing_time_value</t>
   </si>
   <si>
@@ -536,12 +542,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000132</t>
   </si>
   <si>
-    <t>Stored in refrigerator</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000104</t>
-  </si>
-  <si>
     <t>quality_criteria</t>
   </si>
   <si>
@@ -572,7 +572,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-27T18:07:33-07:00</t>
+    <t>2024-02-21T09:25:32-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -674,28 +674,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.5546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="3" width="10.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="6.33984375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="23.45703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="28.5625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="27.40234375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="18.703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="17.54296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="13.0859375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="11.92578125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="23.81640625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="13" width="22.65625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" style="14" width="19.5625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" style="15" width="20.66015625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" style="16" width="21.1484375" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" style="17" width="19.98828125" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="15.8984375" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="15.46875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="14.1875" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="17.671875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="5.94921875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" style="23" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="8.2421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="8.6328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="5.46875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="20.234375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="24.63671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="23.63671875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="16.1328125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="15.1328125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="11.2890625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="10.2890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="20.54296875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="13" width="19.54296875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" style="14" width="16.875" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" style="15" width="17.82421875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" style="16" width="18.2421875" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" style="17" width="17.2421875" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="13.71484375" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="13.34375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="12.23828125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="15.24609375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="5.1328125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -742,16 +742,16 @@
         <v>87</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="S1" t="s" s="1">
         <v>124</v>
@@ -767,7 +767,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="23">
         <v>128</v>
       </c>
     </row>
@@ -805,7 +805,7 @@
       <formula1>'preparation_medium'!$A$1:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_condition'!$A$1:$A$7</formula1>
+      <formula1>'preparation_condition'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -836,90 +836,90 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>89</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>91</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>93</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>95</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>70</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" t="s">
-        <v>119</v>
+      <c r="A6" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>121</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" t="s">
-        <v>121</v>
+      <c r="A7" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>123</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>97</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>99</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" t="s">
-        <v>123</v>
+      <c r="A10" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>78</v>
       </c>
     </row>
@@ -936,37 +936,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.76171875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="79.29296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.0078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="68.3984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>135</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>136</v>
       </c>
     </row>
@@ -984,42 +984,42 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>15</v>
       </c>
     </row>
@@ -1037,34 +1037,34 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>25</v>
       </c>
     </row>
@@ -1082,34 +1082,34 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>35</v>
       </c>
     </row>
@@ -1127,18 +1127,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>41</v>
       </c>
     </row>
@@ -1156,178 +1156,178 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>52</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>54</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>56</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>58</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>60</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>62</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>64</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>66</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>68</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>70</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>72</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>74</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>76</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>78</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>80</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>82</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>84</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>86</v>
       </c>
     </row>
@@ -1338,66 +1338,74 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>89</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>91</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>93</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>95</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>70</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>97</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>99</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1414,26 +1422,26 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>15</v>
       </c>
     </row>
@@ -1451,146 +1459,146 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
+      <c r="A2" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>106</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
+      <c r="A5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
+      <c r="A6" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>108</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>58</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>66</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
+      <c r="A9" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>110</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>70</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
+      <c r="A11" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>112</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" t="s">
-        <v>112</v>
+      <c r="A12" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>114</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>74</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" t="s">
-        <v>114</v>
+      <c r="A14" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>116</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" t="s">
-        <v>116</v>
+      <c r="A15" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>118</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>78</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>84</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new categorical values for preparation medium and storage medium
Closes #9
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="147">
   <si>
     <t>source_id</t>
   </si>
@@ -299,6 +299,90 @@
     <t>preparation_medium</t>
   </si>
   <si>
+    <t>NBF (Neutral Buffered Formalin)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBIB_0000213</t>
+  </si>
+  <si>
+    <t>Allprotect tissue reagent (ALL)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000118</t>
+  </si>
+  <si>
+    <t>CLARITY hydrogel</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000134</t>
+  </si>
+  <si>
+    <t>Trumps fixative</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000331</t>
+  </si>
+  <si>
+    <t>Inflated (OCT)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000123</t>
+  </si>
+  <si>
+    <t>DMEM</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C185409</t>
+  </si>
+  <si>
+    <t>PFA (Paraformaldehyde)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_61538</t>
+  </si>
+  <si>
+    <t>Fixed frozen OCT (Formalin, sucrose protected)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000116</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Fresh frozen OCT</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000126</t>
+  </si>
+  <si>
+    <t>2% PFA/2.5% Glutaraldehyde</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000332</t>
+  </si>
+  <si>
+    <t>Bouin's</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000140</t>
+  </si>
+  <si>
+    <t>Methanol</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_17790</t>
+  </si>
+  <si>
+    <t>PAXgene tissue kit (PXT)</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C185113</t>
+  </si>
+  <si>
     <t>PBS</t>
   </si>
   <si>
@@ -311,24 +395,6 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
   </si>
   <si>
-    <t>Allprotect tissue reagent (ALL)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000118</t>
-  </si>
-  <si>
-    <t>CLARITY hydrogel</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000134</t>
-  </si>
-  <si>
-    <t>Neutral Buffered Formalin (NBF)</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBIB_0000213</t>
-  </si>
-  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -353,48 +419,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000130</t>
   </si>
   <si>
-    <t>Inflated (OCT)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000123</t>
-  </si>
-  <si>
     <t>Fresh frozen gelatin</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000198</t>
   </si>
   <si>
-    <t>PFA (Paraformaldehyde)</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_61538</t>
-  </si>
-  <si>
-    <t>Fixed frozen OCT (Formalin, sucrose protected)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000116</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
-    <t>Fresh frozen OCT</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000126</t>
-  </si>
-  <si>
     <t>RNAlater</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63348</t>
   </si>
   <si>
+    <t>Biops buffer</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000330</t>
+  </si>
+  <si>
     <t>Fixed frozen OCT (Cytofix/Cytoperm)</t>
   </si>
   <si>
@@ -407,30 +449,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C41132</t>
   </si>
   <si>
-    <t>Bouin's</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000140</t>
-  </si>
-  <si>
     <t>Fixed frozen OCT (PFA, sucrose protected)</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000147</t>
   </si>
   <si>
-    <t>Methanol</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_17790</t>
-  </si>
-  <si>
-    <t>PAXgene tissue kit (PXT)</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C185113</t>
-  </si>
-  <si>
     <t>preparation_condition</t>
   </si>
   <si>
@@ -515,6 +539,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000125</t>
   </si>
   <si>
+    <t>Cyro-EM</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000333</t>
+  </si>
+  <si>
     <t>FFPE (Paraffin embedded)</t>
   </si>
   <si>
@@ -572,7 +602,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-02-21T09:25:32-08:00</t>
+    <t>2024-03-12T09:42:58-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -739,36 +769,36 @@
         <v>42</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -802,7 +832,7 @@
       <formula1>'pathology_distance_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$22</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$8</formula1>
@@ -815,7 +845,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$18</formula1>
+      <formula1>'storage_medium'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$11</formula1>
@@ -837,90 +867,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -944,30 +974,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1179,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1329,6 +1359,38 @@
       </c>
       <c r="B22" t="s" s="0">
         <v>86</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1346,66 +1408,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1452,7 +1514,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1460,146 +1522,162 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>44</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>48</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>78</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>86</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typo 'Cyro-EM' to 'Cryo-EM'
Closes #9
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -533,18 +533,18 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65802</t>
   </si>
   <si>
+    <t>Cryo-EM</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000333</t>
+  </si>
+  <si>
     <t>DMSO (serum)</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000125</t>
   </si>
   <si>
-    <t>Cyro-EM</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000333</t>
-  </si>
-  <si>
     <t>FFPE (Paraffin embedded)</t>
   </si>
   <si>
@@ -602,7 +602,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-12T09:42:58-07:00</t>
+    <t>2024-03-14T10:54:38-04:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1618,18 +1618,18 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
Added new preparation mediums
Closes #21
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
   <si>
     <t>source_id</t>
   </si>
@@ -359,6 +359,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000126</t>
   </si>
   <si>
+    <t>Alpha-MEM</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000371</t>
+  </si>
+  <si>
     <t>2% PFA/2.5% Glutaraldehyde</t>
   </si>
   <si>
@@ -395,6 +401,12 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
   </si>
   <si>
+    <t>Modified Davidson's Fixative</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000370</t>
+  </si>
+  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -425,6 +437,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000198</t>
   </si>
   <si>
+    <t>Growth media</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000372</t>
+  </si>
+  <si>
     <t>RNAlater</t>
   </si>
   <si>
@@ -602,7 +620,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-18T09:38:56-07:00</t>
+    <t>2024-03-22T17:02:47-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -769,36 +787,36 @@
         <v>42</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +850,7 @@
       <formula1>'pathology_distance_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$26</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$29</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$8</formula1>
@@ -867,34 +885,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
@@ -907,50 +925,50 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -974,30 +992,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1197,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1391,6 +1409,30 @@
       </c>
       <c r="B26" t="s" s="0">
         <v>94</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1408,34 +1450,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
@@ -1448,26 +1490,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1522,18 +1564,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
@@ -1546,10 +1588,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
@@ -1562,18 +1604,18 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
@@ -1586,10 +1628,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10">
@@ -1602,82 +1644,82 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 'Stored in desiccator' as a new storage method
Closes #45
Note: Sample section is already updated by the previous commit
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="161">
   <si>
     <t>source_id</t>
   </si>
@@ -230,6 +230,12 @@
     <t>http://purl.obolibrary.org/obo/UO_0000023</t>
   </si>
   <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000021</t>
+  </si>
+  <si>
     <t>mg</t>
   </si>
   <si>
@@ -242,12 +248,6 @@
     <t>http://purl.obolibrary.org/obo/UO_0000009</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000021</t>
-  </si>
-  <si>
     <t>volume_value</t>
   </si>
   <si>
@@ -260,18 +260,18 @@
     <t>http://purl.obolibrary.org/obo/UO_0000097</t>
   </si>
   <si>
+    <t>mm^3</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000136</t>
+  </si>
+  <si>
     <t>um^3</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000112</t>
   </si>
   <si>
-    <t>mm^3</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000136</t>
-  </si>
-  <si>
     <t>ml</t>
   </si>
   <si>
@@ -407,6 +407,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000370</t>
   </si>
   <si>
+    <t>HPMC-PVP</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000386</t>
+  </si>
+  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -473,6 +479,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000147</t>
   </si>
   <si>
+    <t>Lysis buffer</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C178573</t>
+  </si>
+  <si>
     <t>preparation_condition</t>
   </si>
   <si>
@@ -533,6 +545,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
   </si>
   <si>
+    <t>Formic acid in water</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83719</t>
+  </si>
+  <si>
     <t>DMSO (no serum)</t>
   </si>
   <si>
@@ -578,6 +596,12 @@
     <t>storage_method</t>
   </si>
   <si>
+    <t>Stored in desiccator</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000387</t>
+  </si>
+  <si>
     <t>Incubated at 37 degrees celsius</t>
   </si>
   <si>
@@ -620,7 +644,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-22T17:02:47-07:00</t>
+    <t>2024-06-28T15:47:59-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -787,36 +811,36 @@
         <v>42</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +874,7 @@
       <formula1>'pathology_distance_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$29</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$31</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$8</formula1>
@@ -863,10 +887,10 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$20</formula1>
+      <formula1>'storage_medium'!$A$1:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_method'!$A$1:$A$11</formula1>
+      <formula1>'storage_method'!$A$1:$A$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -877,7 +901,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -885,34 +909,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -925,50 +949,58 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>111</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>98</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -992,30 +1024,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1197,7 +1229,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1433,6 +1465,22 @@
       </c>
       <c r="B29" t="s" s="0">
         <v>100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1450,34 +1498,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
@@ -1490,26 +1538,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1556,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1572,10 +1620,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
@@ -1604,121 +1652,137 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>56</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>127</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>128</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>92</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>98</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>66</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B22" t="s" s="0">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new preparation medium, storage medium and suspension entity type
It seems these changes are for sample metadata schemas instead of RNAseq w/ Probe metadata schema.

The final additions:
- "1X fixation & permeabilization buffer" as a new preparation medium
- "1X quench buffer" as a new storage medium
- "Nucleus + cell" as a new suspension entity type

Closes #77
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="167">
   <si>
     <t>source_id</t>
   </si>
@@ -323,6 +323,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000331</t>
   </si>
   <si>
+    <t>1X fixation &amp; permeabilization buffer</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000425</t>
+  </si>
+  <si>
     <t>Inflated (OCT)</t>
   </si>
   <si>
@@ -539,6 +545,12 @@
     <t>storage_medium</t>
   </si>
   <si>
+    <t>1X quench buffer</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000427</t>
+  </si>
+  <si>
     <t>OCT</t>
   </si>
   <si>
@@ -563,6 +575,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000135</t>
   </si>
   <si>
+    <t>Concentrated quench buffer</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000391</t>
+  </si>
+  <si>
     <t>Gelatin</t>
   </si>
   <si>
@@ -644,7 +662,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-06-28T15:47:59-07:00</t>
+    <t>2025-03-27T10:36:03-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -811,36 +829,36 @@
         <v>42</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +892,7 @@
       <formula1>'pathology_distance_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$31</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$32</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$8</formula1>
@@ -887,7 +905,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$22</formula1>
+      <formula1>'storage_medium'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$12</formula1>
@@ -909,98 +927,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1024,30 +1042,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1247,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1481,6 +1499,14 @@
       </c>
       <c r="B31" t="s" s="0">
         <v>104</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1498,66 +1524,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1630,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1612,178 +1638,194 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>44</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>46</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>126</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>80</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>128</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>86</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>130</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>60</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>134</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>94</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>100</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>65</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>66</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B23" t="s" s="0">
         <v>72</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update other sample metadata templates
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -30,137 +30,157 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier for the source (parent) from which
-the sample was taken. Example: HBM122.EFGH.789 or SNT234.RTYU.119</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the source (parent
+data) from which the sample was derived. Example: HBM122.EFGH.789</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier for the sample assigned by the
-ingest portal. Example: HBM743.CKJW.876 or SNT923.UYTE.122</t>
+        <t>(Required) The unique HuBMAP or SenNet identifier assigned to the sample by the
+ingest portal. Example: HBM743.CKJW.876</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>The weight of a tissue block or the piece of tissue used in a suspension.
-Knowing the weight of the parent block and tissue used in a suspension, allows
-us to compute what percentage of the block was used for the suspension.</t>
+        <t>The weight of a tissue block or the piece of tissue used in a suspension. This
+information is crucial for calculating the percentage of the parent block that
+was utilized in the suspension preparation. If the weight is not applicable or
+unknown, this field may be left blank. Example: 100</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>The tissue weight unit of measurement</t>
+        <t>The unit of measurement for the tissue weight value. If no tissue weight is
+specified, this field may be left blank. Example: g</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>The volume of the sample block</t>
+        <t>The volume of the object in question. Example: 102</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>The volume unit of measurement</t>
+        <t>The unit of measurement for the volume value. If no volume measurement is
+specified, this field may be left blank. Example: mm^3</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>If a surgical sample, how far from the pathology was the sample obtained.</t>
+        <t>The distance from which the surgical sample was obtained relative to the
+pathology site. If this information is not applicable, this field may be left
+blank. Example: 100</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The distance unit of measurement</t>
+        <t>The unit of measurement for the pathology distance value. If no distance
+measurement is applicable, this field may be left blank. Example: mm</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The medium used during the sample preparation</t>
+        <t>(Required) The medium used during the sample preparation process. If no specific
+medium was utilized, enter "None". If medium was not recorded, enter "Unknown".
+Example: Fresh frozen CMC</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The condition by which the preparation occurred, such as was the
-sample placed in dry ice during the preparation.</t>
+        <t>(Required) The condition under which the sample preparation took place, such as
+whether the sample was placed on dry ice during the process. If preparation
+condition was not recorded, enter "Unknown". Example: Frozen on dry ice</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>How long the tissue was being handled before the initial preservation</t>
+        <t>The duration for which the tissue was handled prior to its initial preservation.
+Example: 120</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement for the processing time value. If processing time is not
+specified, this field may be left blank. Example: minute</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) What was the sample preserved in.</t>
+        <t>(Required) The medium used to preserve the sample. If no specific medium was
+utilized, enter "None". If medium was not recorded, enter "Unknown". Example:
+FFPE (Paraffin embedded)</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) The method by which the sample was stored, after preparation and
-before the assay was performed.</t>
+        <t>(Required) The method used to store the sample after preparation and prior to
+performing the assay. If no specific storage method was utilized, enter "None".
+If storage method was not recorded, enter "Unknown". Example: Frozen in dry ice</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>For example, RIN: 8.7. For suspensions, measured by visual inspection prior to
-cell lysis or defined by known parameters such as wells with several cells or no
-cells. This can be captured at a high level. "OK" or "not OK", or with more
-specificity such as "debris", "clump", "low clump".</t>
+        <t>The quality criteria used to assess the sample, which may include metrics such
+as RIN (e.g., RIN: 8.7) or visual inspection parameters for suspensions prior to
+cell lysis. These criteria can be captured at a high level with general terms
+like "OK" or "not OK" or with more specific descriptors such as "debris" "clump"
+or "low clump". Example: RIN: 8.7, low clump, no visible debris</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>Histopathological reporting of key variables that are important for the tissue
-(absence of necrosis, comment on composition, significant pathology description,
-high level inflammation/fibrosis assessment, etc.)</t>
+        <t>The key variables in the histopathological report that are crucial for assessing
+the tissue, including the absence of necrosis, comments on tissue composition,
+descriptions of significant pathology, and high-level assessments of
+inflammation or fibrosis. Example: No necrosis observed; tissue composed
+predominantly of hepatocytes with mild portal inflammation and minimal fibrosis</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>Miscellaneous details about the sample, not captured in the existing metadata
-fields.</t>
+        <t>Miscellaneous details about the sample that are not captured in the existing
+metadata fields. Example: Sample was stored at 4°C for 48 hours prior to
+processing due to equipment maintenance delay</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
-processing.</t>
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
+processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
   </commentList>
@@ -168,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="169">
   <si>
     <t>source_id</t>
   </si>
@@ -545,30 +565,54 @@
     <t>storage_medium</t>
   </si>
   <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65147</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
+  </si>
+  <si>
+    <t>DMSO (no serum)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000115</t>
+  </si>
+  <si>
+    <t>Gelatin</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65802</t>
+  </si>
+  <si>
+    <t>DMSO (serum)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000125</t>
+  </si>
+  <si>
+    <t>CMC</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83594</t>
+  </si>
+  <si>
     <t>1X quench buffer</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000427</t>
   </si>
   <si>
-    <t>OCT</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
-  </si>
-  <si>
     <t>Formic acid in water</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83719</t>
   </si>
   <si>
-    <t>DMSO (no serum)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000115</t>
-  </si>
-  <si>
     <t>Tris-EDTA</t>
   </si>
   <si>
@@ -581,36 +625,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000391</t>
   </si>
   <si>
-    <t>Gelatin</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65802</t>
-  </si>
-  <si>
     <t>Cryo-EM</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000333</t>
   </si>
   <si>
-    <t>DMSO (serum)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000125</t>
-  </si>
-  <si>
     <t>FFPE (Paraffin embedded)</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C143028</t>
   </si>
   <si>
-    <t>CMC</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83594</t>
-  </si>
-  <si>
     <t>storage_method</t>
   </si>
   <si>
@@ -662,7 +688,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-04-24T10:45:34-07:00</t>
+    <t>2025-10-16T07:27:32-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -841,24 +867,24 @@
         <v>124</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -905,7 +931,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$24</formula1>
+      <formula1>'storage_medium'!$A$1:$A$25</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$12</formula1>
@@ -967,26 +993,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9">
@@ -1042,30 +1068,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1630,7 +1656,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1638,114 +1664,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>76</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>78</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>130</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>82</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>88</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>134</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>136</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -1758,74 +1784,82 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>139</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>140</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>144</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>102</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>68</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>72</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>74</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new preparation condition and mediums
Closes #125, #126
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="175">
   <si>
     <t>source_id</t>
   </si>
@@ -319,6 +319,12 @@
     <t>preparation_medium</t>
   </si>
   <si>
+    <t>HTK Solution</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000152</t>
+  </si>
+  <si>
     <t>NBF (Neutral Buffered Formalin)</t>
   </si>
   <si>
@@ -451,6 +457,12 @@
     <t>http://purl.bioontology.org/ontology/MESH/C046311</t>
   </si>
   <si>
+    <t>UW Solution</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000151</t>
+  </si>
+  <si>
     <t>MACS tissue storage solution</t>
   </si>
   <si>
@@ -556,6 +568,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000104</t>
   </si>
   <si>
+    <t>Stored on wet ice</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000465</t>
+  </si>
+  <si>
     <t>processing_time_value</t>
   </si>
   <si>
@@ -688,7 +706,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-16T07:27:32-07:00</t>
+    <t>2025-10-21T12:12:55-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -855,36 +873,36 @@
         <v>42</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -918,10 +936,10 @@
       <formula1>'pathology_distance_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$32</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_condition'!$A$1:$A$8</formula1>
+      <formula1>'preparation_condition'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -953,98 +971,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1068,30 +1086,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1291,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1535,6 +1553,22 @@
         <v>106</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1542,7 +1576,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1550,66 +1584,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1664,202 +1706,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Perfadex Plus as preparation medium
Closes #128
</commit_message>
<xml_diff>
--- a/sample-block/latest/sample-block.xlsx
+++ b/sample-block/latest/sample-block.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="177">
   <si>
     <t>source_id</t>
   </si>
@@ -367,6 +367,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C185409</t>
   </si>
   <si>
+    <t>Perfadex Plus</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000249</t>
+  </si>
+  <si>
     <t>PFA (Paraformaldehyde)</t>
   </si>
   <si>
@@ -706,7 +712,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-21T13:43:09-07:00</t>
+    <t>2025-11-03T17:31:46-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -873,36 +879,36 @@
         <v>42</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +942,7 @@
       <formula1>'pathology_distance_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$34</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$9</formula1>
@@ -971,98 +977,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1086,30 +1092,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1291,7 +1297,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1567,6 +1573,14 @@
       </c>
       <c r="B34" t="s" s="0">
         <v>110</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1584,74 +1598,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1706,18 +1720,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3">
@@ -1738,170 +1752,170 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>